<commit_message>
Created .exe file to run All-In-One Python script
</commit_message>
<xml_diff>
--- a/All-In-One Python Fall/scan_log.xlsx
+++ b/All-In-One Python Fall/scan_log.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -663,6 +663,50 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2025-09-10 18:49:37</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>879928</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Trunkwala, Alaqmar Kutbuddin</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2025-09-10 18:50:44</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>879928</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Trunkwala, Alaqmar Kutbuddin</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>